<commit_message>
daily burndown chart update
</commit_message>
<xml_diff>
--- a/Burndown Chart/Burndown Chart Caliber Mobile.xlsx
+++ b/Burndown Chart/Burndown Chart Caliber Mobile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiwo\Desktop\Revature Training\May 24th Batch\Project 3\caliber-mobile-docs\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A88074-95ED-49D8-AE82-D0BFB63C5F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EEEBDD-C201-433D-8C23-5C135C0CC659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
   </bookViews>
@@ -452,6 +452,9 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
@@ -1016,6 +1019,9 @@
                 <c:pt idx="1">
                   <c:v>27</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2698,7 +2704,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2746,6 +2752,9 @@
         <v>44406</v>
       </c>
       <c r="B4">
+        <v>27</v>
+      </c>
+      <c r="C4">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made small changes to Sprint Plan and Burndown Chart to reflect changes to in progress User Stories
</commit_message>
<xml_diff>
--- a/Burndown Chart/Burndown Chart Caliber Mobile.xlsx
+++ b/Burndown Chart/Burndown Chart Caliber Mobile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiwo\Desktop\Revature Training\May 24th Batch\Project 3\caliber-mobile-docs\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EEEBDD-C201-433D-8C23-5C135C0CC659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C62D73-5296-4CB4-8E78-27C99ECA4650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
+    <workbookView xWindow="2136" yWindow="1632" windowWidth="17280" windowHeight="8964" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,25 +305,25 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -870,25 +870,25 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -2704,7 +2704,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2795,7 +2795,7 @@
         <v>44411</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2803,7 +2803,7 @@
         <v>44412</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2811,7 +2811,7 @@
         <v>44413</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2819,7 +2819,7 @@
         <v>44414</v>
       </c>
       <c r="B12">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2827,7 +2827,7 @@
         <v>44415</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2835,7 +2835,7 @@
         <v>44416</v>
       </c>
       <c r="B14">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -2843,7 +2843,7 @@
         <v>44417</v>
       </c>
       <c r="B15">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
edited story points in planning doc, edited story points in burndown chart to reflect stretch goals and currently completed user stories
</commit_message>
<xml_diff>
--- a/Burndown Chart/Burndown Chart Caliber Mobile.xlsx
+++ b/Burndown Chart/Burndown Chart Caliber Mobile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiwo\Desktop\Revature Training\May 24th Batch\Project 3\caliber-mobile-docs\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B25B1E9-7BB8-4FB9-BBBA-B342ABD25DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73C2F5A-2E2A-4EA9-8552-2DA35562F1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2136" yWindow="1632" windowWidth="17280" windowHeight="8964" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,55 +284,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -449,25 +449,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -861,55 +864,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,25 +1029,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2728,7 +2734,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2754,10 +2760,10 @@
         <v>44404</v>
       </c>
       <c r="B2">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2765,10 +2771,10 @@
         <v>44405</v>
       </c>
       <c r="B3">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2776,10 +2782,10 @@
         <v>44406</v>
       </c>
       <c r="B4">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2787,10 +2793,10 @@
         <v>44407</v>
       </c>
       <c r="B5">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C5">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2798,10 +2804,10 @@
         <v>44408</v>
       </c>
       <c r="B6">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2809,10 +2815,10 @@
         <v>44409</v>
       </c>
       <c r="B7">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C7">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2820,10 +2826,10 @@
         <v>44410</v>
       </c>
       <c r="B8">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2831,7 +2837,10 @@
         <v>44411</v>
       </c>
       <c r="B9">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2839,7 +2848,7 @@
         <v>44412</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2847,7 +2856,7 @@
         <v>44413</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2855,7 +2864,7 @@
         <v>44414</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2863,7 +2872,7 @@
         <v>44415</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2871,7 +2880,7 @@
         <v>44416</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -2879,7 +2888,7 @@
         <v>44417</v>
       </c>
       <c r="B15">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -2887,7 +2896,7 @@
         <v>44418</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -2895,7 +2904,7 @@
         <v>44419</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -2903,7 +2912,7 @@
         <v>44420</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated Sprint Plan doc to include sprint review and stretch goals. Updated Burndown Chart to reflect currently completed User Stories and stretch goal Story Points.
</commit_message>
<xml_diff>
--- a/Burndown Chart/Burndown Chart Caliber Mobile.xlsx
+++ b/Burndown Chart/Burndown Chart Caliber Mobile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiwo\Desktop\Revature Training\May 24th Batch\Project 3\caliber-mobile-docs\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73C2F5A-2E2A-4EA9-8552-2DA35562F1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262E37AF-4EB2-4E62-8184-D7FE69B44E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
   </bookViews>
@@ -470,7 +470,7 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1050,7 +1050,7 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2734,7 +2734,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2840,7 +2840,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>